<commit_message>
gui changes, now using pqty
</commit_message>
<xml_diff>
--- a/schedule.xlsx
+++ b/schedule.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23760" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23760" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="58">
   <si>
     <t>Names</t>
   </si>
@@ -182,20 +182,29 @@
     <t>kicker dribbler and lobber</t>
   </si>
   <si>
-    <t>first submission</t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
     <t>camera choice</t>
+  </si>
+  <si>
+    <t>in pogress</t>
+  </si>
+  <si>
+    <t>Gui devlopement</t>
+  </si>
+  <si>
+    <t>first CB submission</t>
+  </si>
+  <si>
+    <t>submission</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -218,15 +227,8 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="9">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -275,6 +277,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -448,7 +456,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -476,7 +484,10 @@
     <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -759,18 +770,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P37"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B21" sqref="B21"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="M3" sqref="M3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.5703125" customWidth="1"/>
-    <col min="6" max="6" width="18.140625" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.5546875" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -814,7 +825,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="20" t="s">
         <v>14</v>
       </c>
@@ -833,13 +844,13 @@
       <c r="N2" s="1"/>
       <c r="O2" s="2"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B3" s="23" t="s">
         <v>38</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="26" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="E3" s="26"/>
       <c r="F3" s="26"/>
@@ -853,7 +864,7 @@
       <c r="N3" s="3"/>
       <c r="O3" s="4"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B4" s="23" t="s">
         <v>40</v>
       </c>
@@ -871,7 +882,7 @@
       <c r="N4" s="3"/>
       <c r="O4" s="4"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B5" s="23" t="s">
         <v>41</v>
       </c>
@@ -889,7 +900,7 @@
       <c r="N5" s="3"/>
       <c r="O5" s="4"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B6" s="23" t="s">
         <v>37</v>
       </c>
@@ -907,16 +918,16 @@
       <c r="N6" s="3"/>
       <c r="O6" s="4"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B7" s="23" t="s">
-        <v>50</v>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B7" s="30" t="s">
+        <v>55</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" s="3"/>
-      <c r="G7" s="3"/>
-      <c r="H7" s="3"/>
+      <c r="E7" s="28"/>
+      <c r="F7" s="28"/>
+      <c r="G7" s="28"/>
+      <c r="H7" s="28"/>
       <c r="I7" s="3"/>
       <c r="J7" s="3"/>
       <c r="K7" s="3"/>
@@ -925,8 +936,10 @@
       <c r="N7" s="3"/>
       <c r="O7" s="4"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B8" s="23"/>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="B8" s="23" t="s">
+        <v>50</v>
+      </c>
       <c r="C8" s="3"/>
       <c r="D8" s="3"/>
       <c r="E8" s="3"/>
@@ -941,7 +954,7 @@
       <c r="N8" s="3"/>
       <c r="O8" s="4"/>
     </row>
-    <row r="9" spans="1:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="21"/>
       <c r="B9" s="24"/>
       <c r="C9" s="5"/>
@@ -958,7 +971,7 @@
       <c r="N9" s="5"/>
       <c r="O9" s="6"/>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="20" t="s">
         <v>15</v>
       </c>
@@ -977,7 +990,7 @@
       <c r="N10" s="1"/>
       <c r="O10" s="2"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B11" s="23" t="s">
         <v>33</v>
       </c>
@@ -995,7 +1008,7 @@
       <c r="N11" s="3"/>
       <c r="O11" s="4"/>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B12" s="23" t="s">
         <v>42</v>
       </c>
@@ -1003,7 +1016,7 @@
       <c r="D12" s="3"/>
       <c r="E12" s="26"/>
       <c r="F12" s="26" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
@@ -1015,7 +1028,7 @@
       <c r="N12" s="3"/>
       <c r="O12" s="4"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B13" s="23" t="s">
         <v>43</v>
       </c>
@@ -1023,9 +1036,9 @@
       <c r="D13" s="3"/>
       <c r="E13" s="3"/>
       <c r="F13" s="3"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="29"/>
+      <c r="I13" s="29"/>
       <c r="J13" s="3"/>
       <c r="K13" s="3"/>
       <c r="L13" s="3"/>
@@ -1033,7 +1046,7 @@
       <c r="N13" s="3"/>
       <c r="O13" s="4"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B14" s="23" t="s">
         <v>51</v>
       </c>
@@ -1051,7 +1064,7 @@
       <c r="N14" s="3"/>
       <c r="O14" s="4"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B15" s="23" t="s">
         <v>37</v>
       </c>
@@ -1069,7 +1082,7 @@
       <c r="N15" s="3"/>
       <c r="O15" s="4"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B16" s="23" t="s">
         <v>49</v>
       </c>
@@ -1077,7 +1090,7 @@
       <c r="D16" s="3"/>
       <c r="E16" s="3"/>
       <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
+      <c r="G16" s="29"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
@@ -1087,7 +1100,7 @@
       <c r="N16" s="3"/>
       <c r="O16" s="4"/>
     </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B17" s="23" t="s">
         <v>50</v>
       </c>
@@ -1105,7 +1118,7 @@
       <c r="N17" s="3"/>
       <c r="O17" s="4"/>
     </row>
-    <row r="18" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="21"/>
       <c r="B18" s="24"/>
       <c r="C18" s="5"/>
@@ -1122,7 +1135,7 @@
       <c r="N18" s="5"/>
       <c r="O18" s="6"/>
     </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A19" s="20" t="s">
         <v>16</v>
       </c>
@@ -1141,14 +1154,16 @@
       <c r="N19" s="1"/>
       <c r="O19" s="2"/>
     </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B20" s="23" t="s">
         <v>30</v>
       </c>
       <c r="C20" s="3"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
+      <c r="D20" s="28" t="s">
+        <v>54</v>
+      </c>
+      <c r="E20" s="27"/>
+      <c r="F20" s="27"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="3"/>
@@ -1159,9 +1174,9 @@
       <c r="N20" s="3"/>
       <c r="O20" s="4"/>
     </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B21" s="23" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C21" s="3"/>
       <c r="D21" s="3"/>
@@ -1177,7 +1192,7 @@
       <c r="N21" s="3"/>
       <c r="O21" s="4"/>
     </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B22" s="23" t="s">
         <v>31</v>
       </c>
@@ -1195,7 +1210,7 @@
       <c r="N22" s="3"/>
       <c r="O22" s="4"/>
     </row>
-    <row r="23" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B23" s="24" t="s">
         <v>32</v>
       </c>
@@ -1213,7 +1228,7 @@
       <c r="N23" s="5"/>
       <c r="O23" s="6"/>
     </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A24" s="20" t="s">
         <v>17</v>
       </c>
@@ -1232,14 +1247,16 @@
       <c r="N24" s="1"/>
       <c r="O24" s="2"/>
     </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B25" s="23" t="s">
         <v>34</v>
       </c>
       <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
+      <c r="D25" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
       <c r="I25" s="3"/>
@@ -1250,14 +1267,16 @@
       <c r="N25" s="3"/>
       <c r="O25" s="4"/>
     </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B26" s="23" t="s">
         <v>35</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
+      <c r="F26" s="27" t="s">
+        <v>57</v>
+      </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
@@ -1268,15 +1287,15 @@
       <c r="N26" s="3"/>
       <c r="O26" s="4"/>
     </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B27" s="23" t="s">
         <v>36</v>
       </c>
       <c r="C27" s="3"/>
       <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="E27" s="27"/>
+      <c r="F27" s="27"/>
+      <c r="G27" s="27"/>
       <c r="H27" s="3"/>
       <c r="I27" s="3"/>
       <c r="J27" s="3"/>
@@ -1286,7 +1305,7 @@
       <c r="N27" s="3"/>
       <c r="O27" s="4"/>
     </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B28" s="23" t="s">
         <v>39</v>
       </c>
@@ -1295,9 +1314,9 @@
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
       <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
+      <c r="H28" s="27"/>
+      <c r="I28" s="27"/>
+      <c r="J28" s="27"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
       <c r="M28" s="3"/>
@@ -1305,7 +1324,7 @@
       <c r="O28" s="4"/>
       <c r="P28" s="17"/>
     </row>
-    <row r="29" spans="1:16" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="21"/>
       <c r="B29" s="24"/>
       <c r="C29" s="5"/>
@@ -1322,7 +1341,7 @@
       <c r="N29" s="5"/>
       <c r="O29" s="6"/>
     </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B30" s="19" t="s">
         <v>18</v>
       </c>
@@ -1330,7 +1349,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B31" s="18" t="s">
         <v>22</v>
       </c>
@@ -1340,7 +1359,7 @@
       <c r="F31" s="7"/>
       <c r="G31" s="7"/>
     </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:16" x14ac:dyDescent="0.3">
       <c r="B32" s="18" t="s">
         <v>21</v>
       </c>
@@ -1351,7 +1370,7 @@
       <c r="I32" s="8"/>
       <c r="J32" s="8"/>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B33" s="18" t="s">
         <v>24</v>
       </c>
@@ -1363,7 +1382,7 @@
       <c r="L33" s="9"/>
       <c r="M33" s="9"/>
     </row>
-    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B34" s="18" t="s">
         <v>25</v>
       </c>
@@ -1374,7 +1393,7 @@
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
     </row>
-    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.3">
       <c r="B35" s="18" t="s">
         <v>26</v>
       </c>
@@ -1384,8 +1403,8 @@
       <c r="N35" s="14"/>
       <c r="O35" s="14"/>
     </row>
-    <row r="36" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="37" spans="2:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="37" spans="2:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>44</v>
       </c>
@@ -1404,6 +1423,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>